<commit_message>
Fix some function & change data
CheckAllPositive and CheckAllNegative
Data change from Vietnamese to English for easy work :)
</commit_message>
<xml_diff>
--- a/ID3/Resource/data.xlsx
+++ b/ID3/Resource/data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aerospire/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aerospire\Documents\Visual Studio 2013\AnotherID3\ID3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="1720" windowWidth="26720" windowHeight="14900" tabRatio="500"/>
+    <workbookView xWindow="13185" yWindow="1725" windowWidth="26715" windowHeight="14895" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -24,60 +24,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>TT</t>
   </si>
   <si>
-    <t>Màu tóc</t>
-  </si>
-  <si>
-    <t>Chiều cao</t>
-  </si>
-  <si>
-    <t>Cân nặng</t>
-  </si>
-  <si>
-    <t>Dùng thuốc</t>
-  </si>
-  <si>
-    <t>Kết quả</t>
-  </si>
-  <si>
-    <t>Đen</t>
-  </si>
-  <si>
-    <t>Râm</t>
-  </si>
-  <si>
-    <t>Bạc</t>
-  </si>
-  <si>
-    <t>Tầm thước</t>
-  </si>
-  <si>
-    <t>Cao</t>
-  </si>
-  <si>
-    <t>Thấp</t>
-  </si>
-  <si>
-    <t>Nhẹ</t>
-  </si>
-  <si>
-    <t>Vừa phải</t>
-  </si>
-  <si>
-    <t>Nặng</t>
-  </si>
-  <si>
-    <t>Không</t>
-  </si>
-  <si>
-    <t>Có</t>
-  </si>
-  <si>
-    <t>Bị rám</t>
+    <t>HairColor</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Heavy</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Tall</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Cream</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -88,7 +82,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -125,6 +119,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -134,11 +131,11 @@
   <autoFilter ref="A1:F9"/>
   <tableColumns count="6">
     <tableColumn id="1" name="TT"/>
-    <tableColumn id="2" name="Màu tóc"/>
-    <tableColumn id="3" name="Chiều cao"/>
-    <tableColumn id="4" name="Cân nặng"/>
-    <tableColumn id="5" name="Dùng thuốc"/>
-    <tableColumn id="6" name="Kết quả"/>
+    <tableColumn id="2" name="HairColor"/>
+    <tableColumn id="3" name="Height"/>
+    <tableColumn id="4" name="Weight"/>
+    <tableColumn id="5" name="Cream"/>
+    <tableColumn id="6" name="Result"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -410,14 +407,14 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -434,10 +431,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -445,19 +442,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -465,19 +462,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -485,19 +482,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -505,19 +502,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -525,19 +522,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -545,19 +542,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>15</v>
+      <c r="F7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -565,19 +562,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>15</v>
+      <c r="F8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -585,19 +582,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>